<commit_message>
Se añaden archivos sql y excel para facilitar entendimiento de la base de datos
</commit_message>
<xml_diff>
--- a/AGuerrero.TrabajoFinal.DeepSpaceD6/AccionesCartas.xlsx
+++ b/AGuerrero.TrabajoFinal.DeepSpaceD6/AccionesCartas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FP\CENEC\1er año\Programacion\Nuevos Workspaces\ProgramacionEclipse\AGuerrero.TrabajoFinal.DeepSpaceD6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D74E095-36C9-4031-9CDF-CB4CEBDDA41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC030D0-4F60-4AD5-9599-C5D6E211D42F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3913AA5C-A29F-4B7F-BDDA-1CA08A617D06}"/>
   </bookViews>
@@ -19,17 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -423,7 +412,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,74 +430,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>